<commit_message>
Added feature to copy and append list
</commit_message>
<xml_diff>
--- a/.NET Cohort List ID.xlsx
+++ b/.NET Cohort List ID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F86F71-A94F-4C58-91F9-A9C4D38CD87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D4E809-724C-4188-B342-9FA0B6F5FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="12360" yWindow="9375" windowWidth="14580" windowHeight="9570" tabRatio="500" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="4875" yWindow="4560" windowWidth="14580" windowHeight="9570" tabRatio="500" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,39 +26,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <x:si>
-    <x:t>62b68573d5bacf79bd396d8d</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Week 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b6857121e723731dcb07d6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b6856f1b0c9b18e5e84416</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b6856de3108247dbcb359b</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b666a6c9e1e9804b1972b4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>To Do</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b666a6c9e1e9804b1972b5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Doing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b666a6c9e1e9804b1972b6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Done</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <x:si>
+    <x:t>62b74c1db2ceda5fa906598f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thomas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b74c1ebfc68954fbf6f5e5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ying</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b74c20440fb27b11724a3d</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Esther</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b74c21e17fdb80e8513e7a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zaur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b74c23e2197787f1b7e3b4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Diahandra</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -416,21 +413,19 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A2:B6"/>
+  <x:dimension ref="A2:B8"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E4" sqref="E4 E4:E4"/>
-    </x:sheetView>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="17.2725" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="25.8425" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:2">
       <x:c r="A1" s="2" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <x:row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A2" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -438,53 +433,43 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <x:row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A3" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A4" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A5" s="2" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A6" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B7" s="2" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B8" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="B7" s="2" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <x:c r="B8" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Feature to copy Java Requirements list and append to each associate
</commit_message>
<xml_diff>
--- a/.NET Cohort List ID.xlsx
+++ b/.NET Cohort List ID.xlsx
@@ -26,24 +26,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <x:si>
-    <x:t>62b74c1db2ceda5fa906598f</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thomas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b74c1ebfc68954fbf6f5e5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ying</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62b74c20440fb27b11724a3d</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Esther</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <x:si>
+    <x:t>62b757f7a5d42e8dd3afd466</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Week  1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b7576afe12f938a57c624b</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Diahandra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b666a6bc1aa85d93c63b7f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Doing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b666a6bc1aa85d93c63b80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Done</x:t>
   </x:si>
   <x:si>
     <x:t>62b74c21e17fdb80e8513e7a</x:t>
@@ -53,9 +59,6 @@
   </x:si>
   <x:si>
     <x:t>62b74c23e2197787f1b7e3b4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Diahandra</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -417,52 +420,57 @@
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="25.8425" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <x:sheetFormatPr defaultColWidth="33.659375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
-      <x:c r="A1" s="2" t="s"/>
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
     <x:row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A2" s="2" t="s">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A3" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A4" s="2" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A5" s="2" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <x:c r="A6" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>